<commit_message>
updated code for displaying the new user images
</commit_message>
<xml_diff>
--- a/sample datas/Shopme Sample Users Data/Shopme Sample Users Data.xlsx
+++ b/sample datas/Shopme Sample Users Data/Shopme Sample Users Data.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Spring E-Commerce Course\Dummy Data\Shopme Sample Users Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workshopme1\sample datas\Shopme Sample Users Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734A73D8-50DB-4F2A-A2E9-A3E996D9AA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="8460"/>
+    <workbookView minimized="1" xWindow="11700" yWindow="4080" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="2" r:id="rId1"/>
     <sheet name="Users" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Users!$A$4:$H$27</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -456,8 +460,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +492,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -512,19 +524,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -802,31 +817,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" customWidth="1"/>
     <col min="3" max="3" width="99" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.7">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +856,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -852,7 +867,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -863,7 +878,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -874,7 +889,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -885,7 +900,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -905,25 +920,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.1796875" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="5" max="5" width="24.7265625" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" customWidth="1"/>
+    <col min="8" max="8" width="36.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.7">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -933,7 +948,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -985,7 +1000,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1011,7 +1026,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1037,11 +1052,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1063,7 +1078,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1089,7 +1104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -1141,7 +1156,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1167,11 +1182,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>9</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1193,7 +1208,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1219,7 +1234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1245,7 +1260,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1271,7 +1286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -1297,7 +1312,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1323,7 +1338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -1349,11 +1364,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>16</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1375,7 +1390,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -1401,7 +1416,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -1427,7 +1442,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -1453,7 +1468,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -1479,11 +1494,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A25" s="3">
         <v>21</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1505,11 +1520,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A26" s="3">
         <v>22</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1531,7 +1546,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -1557,13 +1572,21 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:H27" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{D8ADFD2B-F7BF-4947-84C7-C1F576F967A4}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{A3AC85B8-EA99-4ADD-8D52-A45B204F94DA}"/>
+    <hyperlink ref="B20" r:id="rId3" xr:uid="{729ABA5F-85EC-4D2E-BCAF-E9CE768432AF}"/>
+    <hyperlink ref="B26" r:id="rId4" xr:uid="{9EF16459-6F63-483F-A47F-279AAC521CD9}"/>
+    <hyperlink ref="B25" r:id="rId5" xr:uid="{2A607192-1156-47FB-9F85-DEC7B01E321F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>